<commit_message>
loader added in sending mail
</commit_message>
<xml_diff>
--- a/flaskr/attendance_sheets/2024/Computer and Information Sciences/Mathematics/2024-04-08.xlsx
+++ b/flaskr/attendance_sheets/2024/Computer and Information Sciences/Mathematics/2024-04-08.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>

</xml_diff>